<commit_message>
Looking at CLalpha in redians
</commit_message>
<xml_diff>
--- a/SpaceFLight/Cal_JavaFoil.xlsx
+++ b/SpaceFLight/Cal_JavaFoil.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\SPACE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Main_Wing" sheetId="1" r:id="rId1"/>
@@ -54,8 +49,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,25 +105,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -419,8 +402,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B303-4FDA-BF44-E228B779123D}"/>
             </c:ext>
@@ -716,35 +698,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B303-4FDA-BF44-E228B779123D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="283234808"/>
-        <c:axId val="283235136"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="68059904"/>
+        <c:axId val="68061440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="283234808"/>
+        <c:axId val="68059904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -779,19 +751,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283235136"/>
+        <c:crossAx val="68061440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="283235136"/>
+        <c:axId val="68061440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -809,7 +779,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -838,7 +807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="283234808"/>
+        <c:crossAx val="68059904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -852,7 +821,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -881,29 +849,18 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -932,12 +889,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1282,35 +1237,25 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-79DA-4474-AD89-57210F2E3915}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="382313656"/>
-        <c:axId val="382313328"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="68086016"/>
+        <c:axId val="68501504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="382313656"/>
+        <c:axId val="68086016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1345,19 +1290,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382313328"/>
+        <c:crossAx val="68501504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="382313328"/>
+        <c:axId val="68501504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1375,7 +1318,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1404,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382313656"/>
+        <c:crossAx val="68086016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1419,7 +1361,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1450,7 +1391,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1479,32 +1419,20 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1532,8 +1460,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
@@ -1602,8 +1529,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
@@ -1645,28 +1571,19 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="376613168"/>
-        <c:axId val="376613496"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="68549248"/>
+        <c:axId val="67506560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="376613168"/>
+        <c:axId val="68549248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1701,19 +1618,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376613496"/>
+        <c:crossAx val="67506560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376613496"/>
+        <c:axId val="67506560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1731,7 +1646,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1760,7 +1674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376613168"/>
+        <c:crossAx val="68549248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1774,7 +1688,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1803,7 +1716,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3530,7 +3443,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect l="29083" t="50997" r="29204" b="27154"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -3547,7 +3460,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns=""/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -3642,7 +3555,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect l="54343" t="51077" r="4608" b="27582"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -3659,7 +3572,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns=""/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -3670,7 +3583,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main_Wing"/>
@@ -4191,7 +4104,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4226,7 +4139,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4403,23 +4316,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4430,256 +4343,256 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <f>0.5*1.225*(0.1268)*5.639215*[1]Main_Wing!C2</f>
         <v>8.1111976026970005E-3</v>
       </c>
       <c r="B2">
-        <f>$A$2/(0.5*1.225*(C2^2)*5.639215)</f>
+        <f t="shared" ref="B2:B33" si="0">$A$2/(0.5*1.225*(C2^2)*5.639215)</f>
         <v>23.483359999999998</v>
       </c>
       <c r="C2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3">
-        <f>$A$2/(0.5*1.225*(C3^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>5.8708399999999994</v>
       </c>
       <c r="C3">
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4">
-        <f>$A$2/(0.5*1.225*(C4^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.6092622222222226</v>
       </c>
       <c r="C4">
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5">
-        <f>$A$2/(0.5*1.225*(C5^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>1.4677099999999998</v>
       </c>
       <c r="C5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6">
-        <f>$A$2/(0.5*1.225*(C6^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.93933439999999968</v>
       </c>
       <c r="C6">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7">
-        <f>$A$2/(0.5*1.225*(C7^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.65231555555555565</v>
       </c>
       <c r="C7">
         <v>0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8">
-        <f>$A$2/(0.5*1.225*(C8^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.47925224489795915</v>
       </c>
       <c r="C8">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9">
-        <f>$A$2/(0.5*1.225*(C9^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.36692749999999996</v>
       </c>
       <c r="C9">
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10">
-        <f>$A$2/(0.5*1.225*(C10^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.28991802469135802</v>
       </c>
       <c r="C10">
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11">
-        <f>$A$2/(0.5*1.225*(C11^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.23483359999999992</v>
       </c>
       <c r="C11">
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12">
-        <f>$A$2/(0.5*1.225*(C12^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.19407735537190082</v>
       </c>
       <c r="C12">
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13">
-        <f>$A$2/(0.5*1.225*(C13^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.16307888888888891</v>
       </c>
       <c r="C13">
         <v>0.12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14">
-        <f>$A$2/(0.5*1.225*(C14^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.13895479289940826</v>
       </c>
       <c r="C14">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15">
-        <f>$A$2/(0.5*1.225*(C15^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.11981306122448979</v>
       </c>
       <c r="C15">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16">
-        <f>$A$2/(0.5*1.225*(C16^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>0.10437048888888889</v>
       </c>
       <c r="C16">
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17">
-        <f>$A$2/(0.5*1.225*(C17^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>9.1731874999999991E-2</v>
       </c>
       <c r="C17">
         <v>0.16</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18">
-        <f>$A$2/(0.5*1.225*(C18^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>8.1257301038062266E-2</v>
       </c>
       <c r="C18">
         <v>0.17</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19">
-        <f>$A$2/(0.5*1.225*(C19^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>7.2479506172839506E-2</v>
       </c>
       <c r="C19">
         <v>0.18</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20">
-        <f>$A$2/(0.5*1.225*(C20^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>6.5050858725761773E-2</v>
       </c>
       <c r="C20">
         <v>0.19</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21">
-        <f>$A$2/(0.5*1.225*(C21^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>5.870839999999998E-2</v>
       </c>
       <c r="C21">
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22">
-        <f>$A$2/(0.5*1.225*(C22^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>5.3250249433106585E-2</v>
       </c>
       <c r="C22">
         <v>0.21</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23">
-        <f>$A$2/(0.5*1.225*(C23^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>4.8519338842975206E-2</v>
       </c>
       <c r="C23">
         <v>0.22</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24">
-        <f>$A$2/(0.5*1.225*(C24^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>4.4391984877126651E-2</v>
       </c>
       <c r="C24">
         <v>0.23</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25">
-        <f>$A$2/(0.5*1.225*(C25^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>4.0769722222222228E-2</v>
       </c>
       <c r="C25">
         <v>0.24</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26">
-        <f>$A$2/(0.5*1.225*(C26^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>3.7573375999999999E-2</v>
       </c>
       <c r="C26">
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27">
-        <f>$A$2/(0.5*1.225*(C27^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>3.4738698224852066E-2</v>
       </c>
       <c r="C27">
         <v>0.26</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="B28">
-        <f>$A$2/(0.5*1.225*(C28^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>3.2213113854595327E-2</v>
       </c>
       <c r="C28">
         <v>0.27</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5">
       <c r="B29">
-        <f>$A$2/(0.5*1.225*(C29^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.9953265306122447E-2</v>
       </c>
       <c r="C29">
@@ -4693,9 +4606,9 @@
         <v>-5.3084990038314107E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5">
       <c r="B30">
-        <f>$A$2/(0.5*1.225*(C30^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.7923139120095124E-2</v>
       </c>
       <c r="C30">
@@ -4709,9 +4622,9 @@
         <v>7.8800000000000009E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5">
       <c r="B31">
-        <f>$A$2/(0.5*1.225*(C31^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.6092622222222223E-2</v>
       </c>
       <c r="C31">
@@ -4725,9 +4638,9 @@
         <v>8.9560000000000004E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5">
       <c r="B32">
-        <f>$A$2/(0.5*1.225*(C32^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.4436378772112383E-2</v>
       </c>
       <c r="C32">
@@ -4741,171 +4654,171 @@
         <v>-1.3999999999999985E-3</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33">
-        <f>$A$2/(0.5*1.225*(C33^2)*5.639215)</f>
+        <f t="shared" si="0"/>
         <v>2.2932968749999998E-2</v>
       </c>
       <c r="C33">
         <v>0.32</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34">
-        <f>$A$2/(0.5*1.225*(C34^2)*5.639215)</f>
+        <f t="shared" ref="B34:B65" si="1">$A$2/(0.5*1.225*(C34^2)*5.639215)</f>
         <v>2.1564150596877864E-2</v>
       </c>
       <c r="C34">
         <v>0.33</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35">
-        <f>$A$2/(0.5*1.225*(C35^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>2.0314325259515566E-2</v>
       </c>
       <c r="C35">
         <v>0.34</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3">
       <c r="B36">
-        <f>$A$2/(0.5*1.225*(C36^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.9170089795918371E-2</v>
       </c>
       <c r="C36">
         <v>0.35</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3">
       <c r="B37">
-        <f>$A$2/(0.5*1.225*(C37^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.8119876543209876E-2</v>
       </c>
       <c r="C37">
         <v>0.36</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3">
       <c r="B38">
-        <f>$A$2/(0.5*1.225*(C38^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.7153659605551496E-2</v>
       </c>
       <c r="C38">
         <v>0.37</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39">
-        <f>$A$2/(0.5*1.225*(C39^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.6262714681440443E-2</v>
       </c>
       <c r="C39">
         <v>0.38</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3">
       <c r="B40">
-        <f>$A$2/(0.5*1.225*(C40^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.5439421433267585E-2</v>
       </c>
       <c r="C40">
         <v>0.39</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3">
       <c r="B41">
-        <f>$A$2/(0.5*1.225*(C41^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.4677099999999995E-2</v>
       </c>
       <c r="C41">
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3">
       <c r="B42">
-        <f>$A$2/(0.5*1.225*(C42^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.3969875074360502E-2</v>
       </c>
       <c r="C42">
         <v>0.41</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3">
       <c r="B43">
-        <f>$A$2/(0.5*1.225*(C43^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.3312562358276646E-2</v>
       </c>
       <c r="C43">
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3">
       <c r="B44">
-        <f>$A$2/(0.5*1.225*(C44^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.2700573282855598E-2</v>
       </c>
       <c r="C44">
         <v>0.43</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3">
       <c r="B45">
-        <f>$A$2/(0.5*1.225*(C45^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.2129834710743801E-2</v>
       </c>
       <c r="C45">
         <v>0.44</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3">
       <c r="B46">
-        <f>$A$2/(0.5*1.225*(C46^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.1596720987654321E-2</v>
       </c>
       <c r="C46">
         <v>0.45</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3">
       <c r="B47">
-        <f>$A$2/(0.5*1.225*(C47^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.1097996219281663E-2</v>
       </c>
       <c r="C47">
         <v>0.46</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3">
       <c r="B48">
-        <f>$A$2/(0.5*1.225*(C48^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.0630765052059754E-2</v>
       </c>
       <c r="C48">
         <v>0.47</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49">
-        <f>$A$2/(0.5*1.225*(C49^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>1.0192430555555557E-2</v>
       </c>
       <c r="C49">
         <v>0.48</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50">
-        <f>$A$2/(0.5*1.225*(C50^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>9.780658059142024E-3</v>
       </c>
       <c r="C50">
         <v>0.49</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51">
-        <f>$A$2/(0.5*1.225*(C51^2)*5.639215)</f>
+        <f t="shared" si="1"/>
         <v>9.3933439999999997E-3</v>
       </c>
       <c r="C51">
@@ -4919,14 +4832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>